<commit_message>
Adicionando novas tabelas ao suplemento
</commit_message>
<xml_diff>
--- a/Artigo 4/Supplementary Appendix A/general_nested_results.xlsx
+++ b/Artigo 4/Supplementary Appendix A/general_nested_results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27dfba7ba8e15536/Área de Trabalho/Material_Suplementar/Artigo 4/Supplementary Appendix A/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27dfba7ba8e15536/Área de Trabalho/Material_Suplementar/Artigo 4 - Copia/Supplementary Appendix A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F93E1D9F-4D41-4337-BCC9-405FF7E40F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{F93E1D9F-4D41-4337-BCC9-405FF7E40F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{413CF51D-6A1A-4053-ADE5-2AE09794DED9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC8A3053-EB0E-4067-88C9-76E3095E820C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC8A3053-EB0E-4067-88C9-76E3095E820C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table A3" sheetId="1" r:id="rId1"/>
+    <sheet name="Table A4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>Table 2. Performance of nested cross-validation for general model without Boruta feature selection.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -56,46 +54,41 @@
     <t>Catboost Regression</t>
   </si>
   <si>
-    <t>0.269</t>
-  </si>
-  <si>
     <t>LightGBM Regression</t>
   </si>
   <si>
-    <t>0.255</t>
-  </si>
-  <si>
     <t>Extra Tree Regression</t>
   </si>
   <si>
-    <t>0.253</t>
-  </si>
-  <si>
     <t>Elastic Net Regression</t>
   </si>
   <si>
-    <t>0.240</t>
-  </si>
-  <si>
     <t>Lasso Regression</t>
   </si>
   <si>
-    <t>0.228</t>
-  </si>
-  <si>
     <t>Xgboost Regression</t>
   </si>
   <si>
-    <t>0.096</t>
-  </si>
-  <si>
     <t>Ridge Regression</t>
+  </si>
+  <si>
+    <t>&lt;0.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table A4. Performance of nested cross-validation without Boruta feature selection. Model with populational filter for 20,000 inhabitants and over. </t>
+  </si>
+  <si>
+    <t>Table A3. Performance of nested cross-validation for general model without Boruta feature selection.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="#,##0.000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -173,17 +166,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +501,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,127 +509,271 @@
     <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="73.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1778410</v>
-      </c>
-      <c r="C3" s="3">
-        <v>42171</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1778.41</v>
+      </c>
+      <c r="C3" s="5">
+        <v>42.170999999999999</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.26900000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1813410</v>
-      </c>
-      <c r="C4" s="3">
-        <v>42584</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1813.41</v>
+      </c>
+      <c r="C4" s="5">
+        <v>42.584000000000003</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.255</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1819328</v>
-      </c>
-      <c r="C5" s="3">
-        <v>42654</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1819.328</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42.654000000000003</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1850057</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43012</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1850.057</v>
+      </c>
+      <c r="C6" s="5">
+        <v>43.012</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1878576</v>
-      </c>
-      <c r="C7" s="3">
-        <v>43343</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1878.576</v>
+      </c>
+      <c r="C7" s="5">
+        <v>43.343000000000004</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.22800000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2199571</v>
-      </c>
-      <c r="C8" s="3">
-        <v>46900</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2199.5709999999999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>46.9</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2200242</v>
-      </c>
-      <c r="C9" s="5">
-        <v>46907</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2200.2420000000002</v>
+      </c>
+      <c r="C9" s="6">
+        <v>46.906999999999996</v>
+      </c>
+      <c r="D9" s="8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C4992C-9BC2-43F3-A6C6-5565A866C2EF}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1288.453</v>
+      </c>
+      <c r="C3" s="2">
+        <v>35.895000000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1298.2249999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>36.030999999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1318.1569999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>36.305999999999997</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1461.018</v>
+      </c>
+      <c r="C6" s="2">
+        <v>38.222999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.27700000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1466.634</v>
+      </c>
+      <c r="C7" s="2">
+        <v>38.296999999999997</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1540.9829999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>39.255000000000003</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2174.8029999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <v>46.634999999999998</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>